<commit_message>
Aoc 2022 - cleanup and optimization - Day1-5
</commit_message>
<xml_diff>
--- a/resources/GraphTraversalBluePrint.xlsx
+++ b/resources/GraphTraversalBluePrint.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="55">
   <si>
     <t>Search Type</t>
   </si>
@@ -189,19 +189,19 @@
     <t>Memo state found in table/cache</t>
   </si>
   <si>
-    <t>Memoization with compressed state</t>
-  </si>
-  <si>
-    <t>Compressed(robots)</t>
-  </si>
-  <si>
-    <t>Compressed(minerals)</t>
-  </si>
-  <si>
     <t>Time/minutes</t>
   </si>
   <si>
     <t>Time depleted</t>
+  </si>
+  <si>
+    <t>MineralCounts</t>
+  </si>
+  <si>
+    <t>RobotCounts</t>
+  </si>
+  <si>
+    <t>Prune excess mineral counts</t>
   </si>
 </sst>
 </file>
@@ -316,7 +316,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -343,7 +343,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -662,16 +661,16 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35" style="17" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.7109375" customWidth="1"/>
     <col min="4" max="4" width="34.42578125" style="10" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" style="10" customWidth="1"/>
     <col min="6" max="6" width="28.42578125" style="10" customWidth="1"/>
     <col min="7" max="7" width="47.5703125" style="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="33.5703125" customWidth="1"/>
@@ -702,7 +701,7 @@
     </row>
     <row r="2" spans="1:8" s="4" customFormat="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="15" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -711,6 +710,7 @@
       <c r="D2" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="E2" s="5"/>
       <c r="F2" s="5" t="s">
         <v>10</v>
       </c>
@@ -723,7 +723,7 @@
     </row>
     <row r="3" spans="1:8" s="4" customFormat="1">
       <c r="A3" s="3"/>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -732,6 +732,7 @@
       <c r="D3" s="5" t="s">
         <v>14</v>
       </c>
+      <c r="E3" s="5"/>
       <c r="F3" s="5" t="s">
         <v>15</v>
       </c>
@@ -744,7 +745,7 @@
     </row>
     <row r="4" spans="1:8" s="4" customFormat="1">
       <c r="A4" s="3"/>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -753,6 +754,7 @@
       <c r="D4" s="5" t="s">
         <v>19</v>
       </c>
+      <c r="E4" s="5"/>
       <c r="F4" s="5" t="s">
         <v>20</v>
       </c>
@@ -760,26 +762,29 @@
     </row>
     <row r="5" spans="1:8" s="4" customFormat="1">
       <c r="A5" s="3"/>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
     </row>
     <row r="6" spans="1:8" s="4" customFormat="1">
       <c r="A6" s="3"/>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>33</v>
       </c>
       <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:8" s="7" customFormat="1">
       <c r="A7" s="6"/>
-      <c r="B7" s="17"/>
+      <c r="B7" s="16"/>
       <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
     </row>
@@ -787,7 +792,7 @@
       <c r="A8" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="17" t="s">
         <v>21</v>
       </c>
       <c r="C8" t="s">
@@ -796,16 +801,16 @@
       <c r="D8" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E8" t="s">
-        <v>53</v>
+      <c r="E8" s="10" t="s">
+        <v>50</v>
       </c>
       <c r="F8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="22" t="s">
+      <c r="G8" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="21" t="s">
+      <c r="H8" s="20" t="s">
         <v>24</v>
       </c>
     </row>
@@ -813,35 +818,35 @@
       <c r="D9" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="10" t="s">
         <v>23</v>
       </c>
       <c r="F9" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="G9" s="22" t="s">
+      <c r="G9" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="H9" s="20"/>
+      <c r="H9" s="19"/>
     </row>
     <row r="10" spans="1:8" ht="30">
       <c r="D10" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="10" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="E11" t="s">
+      <c r="E11" s="10" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="12" customFormat="1">
       <c r="A12" s="11"/>
-      <c r="B12" s="19"/>
+      <c r="B12" s="18"/>
       <c r="D12" s="13"/>
-      <c r="E12" s="12" t="s">
+      <c r="E12" s="13" t="s">
         <v>44</v>
       </c>
       <c r="F12" s="13"/>
@@ -851,7 +856,7 @@
       <c r="A13" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="17" t="s">
         <v>33</v>
       </c>
       <c r="C13" t="s">
@@ -861,10 +866,10 @@
         <v>29</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G13" s="10" t="s">
         <v>11</v>
@@ -874,25 +879,29 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="30">
-      <c r="D14" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>51</v>
+      <c r="D14" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>53</v>
       </c>
       <c r="F14" s="10" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:8">
+      <c r="D15" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="E15" s="14" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="12" customFormat="1">
       <c r="A16" s="11"/>
-      <c r="B16" s="19"/>
+      <c r="B16" s="18"/>
       <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
     </row>
@@ -900,7 +909,7 @@
       <c r="A17" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="17" t="s">
         <v>41</v>
       </c>
       <c r="C17" t="s">
@@ -915,15 +924,15 @@
       <c r="F17" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="G17" s="15" t="s">
+      <c r="G17" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="H17" s="15" t="s">
+      <c r="H17" s="14" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="30">
-      <c r="E18" t="s">
+      <c r="E18" s="10" t="s">
         <v>47</v>
       </c>
       <c r="F18" s="10" t="s">
@@ -932,8 +941,9 @@
     </row>
     <row r="20" spans="1:8" s="12" customFormat="1">
       <c r="A20" s="11"/>
-      <c r="B20" s="19"/>
+      <c r="B20" s="18"/>
       <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
     </row>
@@ -941,7 +951,7 @@
       <c r="A21" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="17" t="s">
         <v>38</v>
       </c>
       <c r="C21" t="s">
@@ -953,13 +963,13 @@
       <c r="E21" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="F21" s="15" t="s">
+      <c r="F21" s="14" t="s">
         <v>37</v>
       </c>
       <c r="G21" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H21" s="15" t="s">
+      <c r="H21" s="14" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>